<commit_message>
added sequence.txt to 1045 in old crypto fastq to match /lts
</commit_message>
<xml_diff>
--- a/old_database/crypto/fastqFiles/fastq_1045.xlsx
+++ b/old_database/crypto/fastqFiles/fastq_1045.xlsx
@@ -46,58 +46,58 @@
     <t xml:space="preserve">Retrofitted_1045</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_TGAGGTT.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_GCTTAGA.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_ATGACAG.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_CACCTCC.fq</t>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_TGAGGTT.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_GCTTAGA.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_ATGACAG.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_CACCTCC.fq</t>
   </si>
   <si>
     <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_ATCGAGC.fq</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_TACTCTA.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_AGACTGA.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_CTTGGAA.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_CCGATTA.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_GGCAGCG.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_CCATCAT.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_TAACAAG.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_GAGGCGT.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_TTTAACT.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_GGTCCTC.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_CGGTGGC.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_ACTGTCG.fq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence_GTATTTG.fq</t>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_TACTCTA.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_AGACTGA.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_CTTGGAA.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_CCGATTA.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_GGCAGCG.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_CCATCAT.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_TAACAAG.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_GAGGCGT.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_TTTAACT.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_GGTCCTC.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_CGGTGGC.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_ACTGTCG.fq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_1045_samples/run_1045_s_7_withindex_sequence.txt_GTATTTG.fq</t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -327,7 +327,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
@@ -367,7 +367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>6</v>
       </c>

</xml_diff>